<commit_message>
Enhance summary export by sorting allowance ranges in descending order
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -468,67 +468,67 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>192.0 - 208.0</t>
+          <t>220.8 - 239.2</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>203.3</v>
+        <v>222.8</v>
       </c>
       <c r="C2" t="n">
-        <v>197.4</v>
+        <v>227.3</v>
       </c>
       <c r="D2" t="n">
-        <v>200.9</v>
+        <v>223.2</v>
       </c>
       <c r="E2" t="n">
-        <v>205.1</v>
+        <v>227</v>
       </c>
       <c r="F2" t="n">
-        <v>200.6</v>
+        <v>221.6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>336.0 - 364.0</t>
+          <t>144.0 - 156.0</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>339</v>
+        <v>147.9</v>
       </c>
       <c r="C3" t="n">
-        <v>342</v>
+        <v>148</v>
       </c>
       <c r="D3" t="n">
-        <v>339.8</v>
+        <v>149.3</v>
       </c>
       <c r="E3" t="n">
-        <v>349.2</v>
+        <v>148.1</v>
       </c>
       <c r="F3" t="n">
-        <v>350.3</v>
+        <v>150.6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>528.0 - 572.0</t>
+          <t>67.2 - 72.8</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>531.8</v>
+        <v>72.8</v>
       </c>
       <c r="C4" t="n">
-        <v>535.8</v>
+        <v>72.8</v>
       </c>
       <c r="D4" t="n">
-        <v>540.8</v>
+        <v>70.90000000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>555.1</v>
+        <v>67.7</v>
       </c>
       <c r="F4" t="n">
-        <v>557.8</v>
+        <v>67.40000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add live torque display and ensure reading emission on all torque values
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -472,19 +472,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>222.8</v>
+        <v>223.9</v>
       </c>
       <c r="C2" t="n">
-        <v>227.3</v>
+        <v>239.2</v>
       </c>
       <c r="D2" t="n">
-        <v>223.2</v>
+        <v>235.4</v>
       </c>
       <c r="E2" t="n">
-        <v>227</v>
+        <v>237.3</v>
       </c>
       <c r="F2" t="n">
-        <v>221.6</v>
+        <v>237.2</v>
       </c>
     </row>
     <row r="3">
@@ -494,19 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>147.9</v>
+        <v>153.8</v>
       </c>
       <c r="C3" t="n">
-        <v>148</v>
+        <v>153.8</v>
       </c>
       <c r="D3" t="n">
-        <v>149.3</v>
+        <v>152.8</v>
       </c>
       <c r="E3" t="n">
-        <v>148.1</v>
+        <v>154.4</v>
       </c>
       <c r="F3" t="n">
-        <v>150.6</v>
+        <v>154.3</v>
       </c>
     </row>
     <row r="4">
@@ -516,19 +516,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>72.8</v>
+        <v>68.90000000000001</v>
       </c>
       <c r="C4" t="n">
-        <v>72.8</v>
+        <v>68.2</v>
       </c>
       <c r="D4" t="n">
-        <v>70.90000000000001</v>
+        <v>69.09999999999999</v>
       </c>
       <c r="E4" t="n">
-        <v>67.7</v>
+        <v>69</v>
       </c>
       <c r="F4" t="n">
-        <v>67.40000000000001</v>
+        <v>69.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add OpenAI settings dialog for API key configuration
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -468,67 +468,67 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>220.8 - 239.2</t>
+          <t>528.0 - 572.0</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>223.9</v>
+        <v>564.5</v>
       </c>
       <c r="C2" t="n">
-        <v>239.2</v>
+        <v>555.9</v>
       </c>
       <c r="D2" t="n">
-        <v>235.4</v>
+        <v>546</v>
       </c>
       <c r="E2" t="n">
-        <v>237.3</v>
+        <v>551.2</v>
       </c>
       <c r="F2" t="n">
-        <v>237.2</v>
+        <v>560.2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>144.0 - 156.0</t>
+          <t>336.0 - 364.0</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>153.8</v>
+        <v>356.7</v>
       </c>
       <c r="C3" t="n">
-        <v>153.8</v>
+        <v>357</v>
       </c>
       <c r="D3" t="n">
-        <v>152.8</v>
+        <v>343.6</v>
       </c>
       <c r="E3" t="n">
-        <v>154.4</v>
+        <v>342.4</v>
       </c>
       <c r="F3" t="n">
-        <v>154.3</v>
+        <v>355.2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>67.2 - 72.8</t>
+          <t>192.0 - 208.0</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>68.90000000000001</v>
+        <v>197.4</v>
       </c>
       <c r="C4" t="n">
-        <v>68.2</v>
+        <v>200.4</v>
       </c>
       <c r="D4" t="n">
-        <v>69.09999999999999</v>
+        <v>199.5</v>
       </c>
       <c r="E4" t="n">
-        <v>69</v>
+        <v>205.3</v>
       </c>
       <c r="F4" t="n">
-        <v>69.3</v>
+        <v>205.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add AppSettings table and functions for managing application settings
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,30 +436,35 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Allowance Range</t>
+          <t>Applied Torque</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Min-Max Allowance</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Test 1</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Test 2</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Test 3</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Test 4</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Test 5</t>
         </is>
@@ -468,67 +473,112 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>528.0 - 572.0</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>564.5</v>
-      </c>
-      <c r="C2" t="n">
-        <v>555.9</v>
-      </c>
-      <c r="D2" t="n">
-        <v>546</v>
-      </c>
-      <c r="E2" t="n">
-        <v>551.2</v>
-      </c>
-      <c r="F2" t="n">
-        <v>560.2</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>544.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>554.3</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>563.2</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>550.7</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>567.1</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>350</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>336.0 - 364.0</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>356.7</v>
-      </c>
-      <c r="C3" t="n">
-        <v>357</v>
-      </c>
-      <c r="D3" t="n">
-        <v>343.6</v>
-      </c>
-      <c r="E3" t="n">
-        <v>342.4</v>
-      </c>
-      <c r="F3" t="n">
-        <v>355.2</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>355.1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>363.0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>355.6</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>359.2</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>349.4</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>192.0 - 208.0</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>197.4</v>
-      </c>
-      <c r="C4" t="n">
-        <v>200.4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>199.5</v>
-      </c>
-      <c r="E4" t="n">
-        <v>205.3</v>
-      </c>
-      <c r="F4" t="n">
-        <v>205.5</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>203.3</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>207.9</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>207.4</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>207.0</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>201.0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor main.py comments, remove unused OpenAI settings dialog and template files
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -483,27 +483,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>544.0</t>
+          <t>556.2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>554.3</t>
+          <t>559.6</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>563.2</t>
+          <t>557.1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>550.7</t>
+          <t>562.0</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>567.1</t>
+          <t>541.3</t>
         </is>
       </c>
     </row>
@@ -520,27 +520,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>355.1</t>
+          <t>363.6</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>363.0</t>
+          <t>345.1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>355.6</t>
+          <t>356.4</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>359.2</t>
+          <t>353.3</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>349.4</t>
+          <t>362.8</t>
         </is>
       </c>
     </row>
@@ -557,27 +557,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>203.3</t>
+          <t>204.5</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>207.9</t>
+          <t>202.7</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>207.4</t>
+          <t>202.4</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>207.0</t>
+          <t>199.5</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>201.0</t>
+          <t>194.6</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor OCR functionality in openai_handler.py to use new OpenAI client interface and improve image handling; clean up serial_reader.py by removing debug print statement
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -483,27 +483,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>556.2</t>
+          <t>567.4</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>559.6</t>
+          <t>562.3</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>557.1</t>
+          <t>562.8</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>562.0</t>
+          <t>564.1</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>541.3</t>
+          <t>563.9</t>
         </is>
       </c>
     </row>
@@ -520,27 +520,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>363.6</t>
+          <t>357.6</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>345.1</t>
+          <t>355.1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>356.4</t>
+          <t>359.6</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>353.3</t>
+          <t>358.0</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>362.8</t>
+          <t>361.0</t>
         </is>
       </c>
     </row>
@@ -557,27 +557,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>204.5</t>
+          <t>196.2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>202.7</t>
+          <t>195.9</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>202.4</t>
+          <t>199.0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>199.5</t>
+          <t>198.8</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>194.6</t>
+          <t>199.9</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update summary.xlsx with latest data revisions
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Min-Max Allowance</t>
+          <t>Min - Max Allowance</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -467,6 +467,56 @@
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Test 5</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturer</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Serial Number</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Calibration Date</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Calibration Due</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Number</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Customer/Company</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Phone Number</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>OCR Text</t>
         </is>
       </c>
     </row>
@@ -483,29 +533,47 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>567.4</t>
+          <t>567.8</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>562.3</t>
+          <t>553.3</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>562.8</t>
+          <t>550.2</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>564.1</t>
+          <t>561.0</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>563.9</t>
-        </is>
-      </c>
+          <t>559.0</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2025-03-03</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2026-03-03</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -520,29 +588,47 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>357.6</t>
+          <t>362.5</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>355.1</t>
+          <t>353.5</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>359.6</t>
+          <t>351.1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>358.0</t>
+          <t>360.8</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>361.0</t>
-        </is>
-      </c>
+          <t>353.5</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2025-03-03</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2026-03-03</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -557,29 +643,47 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>196.2</t>
+          <t>203.3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>195.9</t>
+          <t>200.2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>199.0</t>
+          <t>198.3</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>198.8</t>
+          <t>204.6</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>199.9</t>
-        </is>
-      </c>
+          <t>197.7</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>2025-03-03</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2026-03-03</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactor OCR functionality in modern_torque_app to use new extraction method; update UI to display extracted data in a table format and clean up openai_handler for improved data extraction.
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,46 +514,41 @@
           <t>Address</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>OCR Text</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>230</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>528.0 - 572.0</t>
+          <t>220.8 - 239.2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>567.8</t>
+          <t>227.8</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>553.3</t>
+          <t>231.4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>550.2</t>
+          <t>234.2</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>561.0</t>
+          <t>234.6</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>559.0</t>
+          <t>233.0</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -561,54 +556,53 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-03-03</t>
+          <t>2025-03-05</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2026-03-03</t>
+          <t>2026-03-05</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>350</t>
+          <t>150</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>336.0 - 364.0</t>
+          <t>144.0 - 156.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>362.5</t>
+          <t>145.7</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>353.5</t>
+          <t>151.5</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>351.1</t>
+          <t>154.8</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>360.8</t>
+          <t>148.6</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>353.5</t>
+          <t>149.7</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -616,54 +610,53 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-03-03</t>
+          <t>2025-03-05</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2026-03-03</t>
+          <t>2026-03-05</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>70</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>192.0 - 208.0</t>
+          <t>67.2 - 72.8</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>203.3</t>
+          <t>69.3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>200.2</t>
+          <t>69.9</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>198.3</t>
+          <t>69.8</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>204.6</t>
+          <t>69.9</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>197.7</t>
+          <t>70.2</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
@@ -671,19 +664,18 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-03-03</t>
+          <t>2025-03-05</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2026-03-03</t>
+          <t>2026-03-05</t>
         </is>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Enhance customer info upload options in modern_torque_app; add functionality to upload images from clipboard and webcam, and refactor related methods for improved clarity and usability.
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -518,37 +518,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>230</t>
+          <t>550</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>220.8 - 239.2</t>
+          <t>528.0 - 572.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>227.8</t>
+          <t>565.4</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>231.4</t>
+          <t>556.5</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>234.2</t>
+          <t>554.9</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>234.6</t>
+          <t>560.5</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>233.0</t>
+          <t>556.7</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -572,37 +572,37 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>350</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>144.0 - 156.0</t>
+          <t>336.0 - 364.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>145.7</t>
+          <t>355.7</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>151.5</t>
+          <t>342.1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>154.8</t>
+          <t>343.7</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>148.6</t>
+          <t>341.1</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>149.7</t>
+          <t>339.9</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -626,37 +626,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>200</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>67.2 - 72.8</t>
+          <t>192.0 - 208.0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>69.3</t>
+          <t>200.8</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>69.9</t>
+          <t>195.4</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>69.8</t>
+          <t>193.1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>69.9</t>
+          <t>194.8</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>70.2</t>
+          <t>192.0</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>

</xml_diff>

<commit_message>
Refactor OpenAI extraction logic in openai_handler.py to improve JSON parsing and error handling; update modern_torque_app.py to include QApplication import; update compiled bytecode and summary.xlsx.
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -528,27 +528,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>565.4</t>
+          <t>545.0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>556.5</t>
+          <t>554.3</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>554.9</t>
+          <t>558.7</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>560.5</t>
+          <t>553.1</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>556.7</t>
+          <t>560.8</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -582,27 +582,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>355.7</t>
+          <t>345.7</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>342.1</t>
+          <t>350.2</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>343.7</t>
+          <t>350.9</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>341.1</t>
+          <t>354.2</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>339.9</t>
+          <t>351.8</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -636,27 +636,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>200.8</t>
+          <t>197.7</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>195.4</t>
+          <t>194.5</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>193.1</t>
+          <t>194.0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>194.8</t>
+          <t>192.3</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>192.0</t>
+          <t>192.3</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>

</xml_diff>

<commit_message>
Enhance torque extraction functionality in modern_torque_app and openai_handler; add max_torque and torque_unit fields to JSON response, update UI to display these values, and implement auto-selection logic for torque units.
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -518,42 +518,54 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>230</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>528.0 - 572.0</t>
+          <t>220.8 - 239.2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>545.0</t>
+          <t>234.5</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>554.3</t>
+          <t>235.8</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>558.7</t>
+          <t>235.4</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>553.1</t>
+          <t>236.1</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>560.8</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+          <t>236.6</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>JET</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2408697798</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>JITW-12250 718976</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
           <t>2025-03-05</t>
@@ -564,50 +576,78 @@
           <t>2026-03-05</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>2408697798</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>TIRE CRAFT</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>780-354-2013</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>tracy@tstire.ca</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>350</t>
+          <t>150</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>336.0 - 364.0</t>
+          <t>144.0 - 156.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>345.7</t>
+          <t>147.5</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>350.2</t>
+          <t>154.1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>350.9</t>
+          <t>151.9</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>354.2</t>
+          <t>147.3</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>351.8</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+          <t>152.1</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>JET</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2408697798</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>JITW-12250 718976</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
           <t>2025-03-05</t>
@@ -618,50 +658,78 @@
           <t>2026-03-05</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>2408697798</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>TIRE CRAFT</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>780-354-2013</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>tracy@tstire.ca</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>70</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>192.0 - 208.0</t>
+          <t>67.2 - 72.8</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>197.7</t>
+          <t>69.1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>194.5</t>
+          <t>69.4</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>194.0</t>
+          <t>70.5</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>192.3</t>
+          <t>71.1</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>192.3</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+          <t>72.0</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>JET</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2408697798</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>JITW-12250 718976</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
           <t>2025-03-05</t>
@@ -672,10 +740,26 @@
           <t>2026-03-05</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>2408697798</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>TIRE CRAFT</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>780-354-2013</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>tracy@tstire.ca</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Enhance OpenAI settings management in modern_torque_app; add options for model, temperature, top_p, presence_penalty, and frequency_penalty; implement show/hide functionality for extracted data in the UI.
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -528,27 +528,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>234.5</t>
+          <t>221.6</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>235.8</t>
+          <t>223.8</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>235.4</t>
+          <t>225.7</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>236.1</t>
+          <t>228.5</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>236.6</t>
+          <t>227.7</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -558,12 +558,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2408697798</t>
+          <t>2286916218</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>JITW-12250 718976</t>
+          <t>718976</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -578,24 +578,20 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2408697798</t>
+          <t>TW-78</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>TIRE CRAFT</t>
+          <t>MASTEC CANADA INC.</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>780-354-2013</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>tracy@tstire.ca</t>
-        </is>
-      </c>
+          <t>403-852-5420</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -610,27 +606,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>147.5</t>
+          <t>147.1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>154.1</t>
+          <t>149.1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>151.9</t>
+          <t>149.2</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>147.3</t>
+          <t>148.6</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>152.1</t>
+          <t>148.5</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -640,12 +636,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2408697798</t>
+          <t>2286916218</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>JITW-12250 718976</t>
+          <t>718976</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -660,24 +656,20 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2408697798</t>
+          <t>TW-78</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>TIRE CRAFT</t>
+          <t>MASTEC CANADA INC.</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>780-354-2013</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>tracy@tstire.ca</t>
-        </is>
-      </c>
+          <t>403-852-5420</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -692,27 +684,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>69.1</t>
+          <t>67.9</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>69.4</t>
+          <t>68.0</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>70.5</t>
+          <t>67.3</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>71.1</t>
+          <t>67.4</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>72.0</t>
+          <t>70.0</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -722,12 +714,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2408697798</t>
+          <t>2286916218</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>JITW-12250 718976</t>
+          <t>718976</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -742,24 +734,20 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2408697798</t>
+          <t>TW-78</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>TIRE CRAFT</t>
+          <t>MASTEC CANADA INC.</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>780-354-2013</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>tracy@tstire.ca</t>
-        </is>
-      </c>
+          <t>403-852-5420</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update compiled bytecode and summary file for modern_torque_app
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -528,67 +528,67 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>221.6</t>
+          <t>226.6</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>223.8</t>
+          <t>233.9</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>225.7</t>
+          <t>235.2</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>228.5</t>
+          <t>229.4</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>227.7</t>
+          <t>232.2</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>JET</t>
+          <t>PRECISION INSTRUMENTS</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2286916218</t>
+          <t>145119</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>718976</t>
+          <t>C3FR250F</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-03-05</t>
+          <t>2025-03-06</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2026-03-05</t>
+          <t>2026-03-06</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>TW-78</t>
+          <t>03</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>MASTEC CANADA INC.</t>
+          <t>KALTIRE 089</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>403-852-5420</t>
+          <t>780-228-5970</t>
         </is>
       </c>
       <c r="P2" t="inlineStr"/>
@@ -606,67 +606,67 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>147.1</t>
+          <t>147.5</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>149.1</t>
+          <t>144.3</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>149.2</t>
+          <t>146.5</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>148.6</t>
+          <t>145.7</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>148.5</t>
+          <t>145.7</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>JET</t>
+          <t>PRECISION INSTRUMENTS</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2286916218</t>
+          <t>145119</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>718976</t>
+          <t>C3FR250F</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-03-05</t>
+          <t>2025-03-06</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2026-03-05</t>
+          <t>2026-03-06</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>TW-78</t>
+          <t>03</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>MASTEC CANADA INC.</t>
+          <t>KALTIRE 089</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>403-852-5420</t>
+          <t>780-228-5970</t>
         </is>
       </c>
       <c r="P3" t="inlineStr"/>
@@ -684,67 +684,67 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>67.9</t>
+          <t>72.1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>68.0</t>
+          <t>70.2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>67.3</t>
+          <t>72.1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>67.4</t>
+          <t>71.7</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>70.0</t>
+          <t>71.0</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>JET</t>
+          <t>PRECISION INSTRUMENTS</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2286916218</t>
+          <t>145119</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>718976</t>
+          <t>C3FR250F</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-03-05</t>
+          <t>2025-03-06</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2026-03-05</t>
+          <t>2026-03-06</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>TW-78</t>
+          <t>03</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>MASTEC CANADA INC.</t>
+          <t>KALTIRE 089</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>403-852-5420</t>
+          <t>780-228-5970</t>
         </is>
       </c>
       <c r="P4" t="inlineStr"/>

</xml_diff>

<commit_message>
Update compiled bytecode and summary files for modern_torque_app; add summary_template.xlsx.
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Summary Template" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,320 +422,256 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Applied Torque</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Min - Max Allowance</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Test 1</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Test 2</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Test 3</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Test 4</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Test 5</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Manufacturer</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Serial Number</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Model</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Calibration Date</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Calibration Due</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Unit Number</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Customer/Company</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Phone Number</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Address</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Manufacturer:</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>JET</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>230</t>
+          <t>Serial Number:</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>220.8 - 239.2</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>226.6</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>233.9</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>235.2</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>229.4</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>232.2</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>PRECISION INSTRUMENTS</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>145119</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>C3FR250F</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2025-03-06</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>2026-03-06</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>KALTIRE 089</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>780-228-5970</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr"/>
+          <t>23056350</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>Model:</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>144.0 - 156.0</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>147.5</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>144.3</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>146.5</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>145.7</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>145.7</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>PRECISION INSTRUMENTS</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>145119</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>C3FR250F</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>2025-03-06</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>2026-03-06</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>KALTIRE 089</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>780-228-5970</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr"/>
+          <t>JTW-34600</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>Calibration Date:</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>67.2 - 72.8</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>72.1</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>70.2</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>72.1</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>71.7</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>71.0</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>PRECISION INSTRUMENTS</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>145119</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>C3FR250F</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
           <t>2025-03-06</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Calibration Due:</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>2026-03-06</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>KALTIRE 089</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>780-228-5970</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Unit Number:</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TW-79</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Customer/Company:</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MASTEC CANADA INC.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Phone Number:</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>403-852-5420</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Address:</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Applied Torque</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Min - Max Allowance</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Test 3</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Test 4</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Test 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>528.0 - 572.0</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>566.7</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>568.1</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>571.1</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>566.7</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>564.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>350</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>336.0 - 364.0</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>360.0</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>362.9</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>357.6</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>356.0</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>363.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>192.0 - 208.0</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>203.1</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>201.8</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>202.7</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>204.3</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>201.4</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>